<commit_message>
WIP: improved dataframe for pivot
Improved cumulative value handling and CF taxable payable from standardized_IS_CF.xlsx
</commit_message>
<xml_diff>
--- a/data/standardized_IS_CF.xlsx
+++ b/data/standardized_IS_CF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/Documents/Github/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0D971B-C4BB-E545-89A7-4D75316C5CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977850C6-6901-4345-B048-586FC7344F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="680" windowWidth="21140" windowHeight="20020" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
+    <workbookView xWindow="15780" yWindow="860" windowWidth="21140" windowHeight="20020" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="161">
   <si>
     <t>Revenue</t>
   </si>
@@ -513,6 +513,12 @@
   </si>
   <si>
     <t>CF</t>
+  </si>
+  <si>
+    <t>Increase (Decrease) in Income Taxes Payable</t>
+  </si>
+  <si>
+    <t>(Operating Activities) Change in Accounts Taxes Payable</t>
   </si>
 </sst>
 </file>
@@ -924,15 +930,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="67.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="63.1640625" style="5" customWidth="1"/>
     <col min="3" max="3" width="83.1640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="5" customWidth="1"/>
@@ -1388,7 +1394,7 @@
       <c r="A27" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="7" t="s">
         <v>65</v>
       </c>
       <c r="C27" s="7" t="s">
@@ -1422,7 +1428,7 @@
       <c r="A29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -1471,9 +1477,9 @@
     </row>
     <row r="32" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>77</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -1488,30 +1494,26 @@
     </row>
     <row r="33" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>70</v>
+        <v>160</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>79</v>
+        <v>159</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D33" t="s">
-        <v>151</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>158</v>
-      </c>
+      <c r="D33"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="D34" t="s">
         <v>151</v>
@@ -1522,13 +1524,13 @@
     </row>
     <row r="35" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D35" t="s">
         <v>151</v>
@@ -1539,47 +1541,47 @@
     </row>
     <row r="36" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D36" t="s">
-        <v>151</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
+      <c r="D37" t="s">
+        <v>151</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B38" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="D37" t="s">
-        <v>151</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="D38" t="s">
         <v>151</v>
@@ -1593,10 +1595,10 @@
         <v>93</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D39" t="s">
         <v>151</v>
@@ -1607,13 +1609,13 @@
     </row>
     <row r="40" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D40" t="s">
         <v>151</v>
@@ -1624,13 +1626,13 @@
     </row>
     <row r="41" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D41" t="s">
         <v>151</v>
@@ -1644,10 +1646,10 @@
         <v>101</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D42" t="s">
         <v>151</v>
@@ -1658,13 +1660,13 @@
     </row>
     <row r="43" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D43" t="s">
         <v>151</v>
@@ -1675,13 +1677,13 @@
     </row>
     <row r="44" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D44" t="s">
         <v>151</v>
@@ -1692,47 +1694,47 @@
     </row>
     <row r="45" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B46" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D45" t="s">
-        <v>151</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
+      <c r="D46" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B47" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C47" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="D46" t="s">
-        <v>151</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="D47" t="s">
         <v>151</v>
@@ -1743,13 +1745,13 @@
     </row>
     <row r="48" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D48" t="s">
         <v>151</v>
@@ -1760,13 +1762,13 @@
     </row>
     <row r="49" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D49" t="s">
         <v>151</v>
@@ -1777,13 +1779,13 @@
     </row>
     <row r="50" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D50" t="s">
         <v>151</v>
@@ -1794,13 +1796,13 @@
     </row>
     <row r="51" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D51" t="s">
         <v>151</v>
@@ -1814,27 +1816,27 @@
         <v>130</v>
       </c>
       <c r="B52" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52" t="s">
+        <v>151</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="D52" t="s">
-        <v>151</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>137</v>
       </c>
       <c r="D53" t="s">
         <v>151</v>
@@ -1848,44 +1850,44 @@
         <v>135</v>
       </c>
       <c r="B54" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" t="s">
+        <v>151</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C55" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="D54" t="s">
-        <v>151</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
+      <c r="D55" t="s">
+        <v>151</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C56" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="D55" t="s">
-        <v>151</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="D56" t="s">
         <v>151</v>
@@ -1899,10 +1901,10 @@
         <v>143</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D57" t="s">
         <v>151</v>
@@ -1913,18 +1915,35 @@
     </row>
     <row r="58" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="D58" t="s">
+        <v>151</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>152</v>
       </c>
-      <c r="E58" s="4" t="s">
+      <c r="E59" s="4" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New: utils function to transpose financial statement
</commit_message>
<xml_diff>
--- a/data/standardized_IS_CF.xlsx
+++ b/data/standardized_IS_CF.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/Documents/Github/SEC_data_analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977850C6-6901-4345-B048-586FC7344F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF03E9AA-9B4D-5C4F-9824-F7C49D7CF247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15780" yWindow="860" windowWidth="21140" windowHeight="20020" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="161">
   <si>
     <t>Revenue</t>
   </si>
@@ -932,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1353,7 +1353,7 @@
         <v>151</v>
       </c>
       <c r="E24" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1502,8 +1502,12 @@
       <c r="C33" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D33"/>
-      <c r="E33" s="4"/>
+      <c r="D33" t="s">
+        <v>151</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">

</xml_diff>

<commit_message>
WIP Refactoring handling cumulative val
</commit_message>
<xml_diff>
--- a/data/standardized_IS_CF.xlsx
+++ b/data/standardized_IS_CF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF03E9AA-9B4D-5C4F-9824-F7C49D7CF247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658C2317-2FA8-7B46-9EA4-325E0F7FB22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="860" windowWidth="21140" windowHeight="20020" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
+    <workbookView xWindow="12680" yWindow="6920" windowWidth="21140" windowHeight="20020" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="162">
   <si>
     <t>Revenue</t>
   </si>
@@ -236,9 +236,6 @@
     <t>IncreaseDecreaseInInventories</t>
   </si>
   <si>
-    <t>The increase (decrease) during the reporting period in the aggregate value of all inventory held by the reporting entity, associated with underlying transactions that are classified as operating activities.</t>
-  </si>
-  <si>
     <t>(Operating Activities) Change in Prepaid expenses and other assets</t>
   </si>
   <si>
@@ -482,9 +479,6 @@
     <t>Amount of increase (decrease) in cash and cash equivalents. Cash and cash equivalents are the amount of currency on hand as well as demand deposits with banks or financial institutions. Includes other kinds of accounts that have the general characteristics of demand deposits. Also includes short-term, highly liquid investments that are both readily convertible to known amounts of cash and so near their maturity that they present insignificant risk of changes in value because of changes in interest rates. Includes effect from exchange rate changes.</t>
   </si>
   <si>
-    <t>Cash &amp; Cash Equivalent at the beginning of the period</t>
-  </si>
-  <si>
     <t>CashCashEquivalentsRestrictedCashAndRestrictedCashEquivalents</t>
   </si>
   <si>
@@ -519,6 +513,15 @@
   </si>
   <si>
     <t>(Operating Activities) Change in Accounts Taxes Payable</t>
+  </si>
+  <si>
+    <t>Cash &amp; Cash Equivalent at the  end / beginning of the period</t>
+  </si>
+  <si>
+    <t>AmortizationOfFinancingCostsAndWriteOffOfDeferredDebtIssuanceCos</t>
+  </si>
+  <si>
+    <t>Amortization Of Financing Costs And Write Off Of Deferred Debt Issuance Cost</t>
   </si>
 </sst>
 </file>
@@ -930,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -947,7 +950,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -956,10 +959,10 @@
         <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -974,10 +977,10 @@
         <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -992,10 +995,10 @@
         <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1010,10 +1013,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1027,10 +1030,10 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1044,10 +1047,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1061,10 +1064,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1078,10 +1081,10 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1095,10 +1098,10 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1112,10 +1115,10 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1129,10 +1132,10 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1146,10 +1149,10 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1163,10 +1166,10 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1180,10 +1183,10 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1197,10 +1200,10 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1214,10 +1217,10 @@
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1231,10 +1234,10 @@
         <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1248,10 +1251,10 @@
         <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1265,10 +1268,10 @@
         <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1282,10 +1285,10 @@
         <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1299,10 +1302,10 @@
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1316,10 +1319,10 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1333,10 +1336,10 @@
         <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1350,10 +1353,10 @@
         <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1361,594 +1364,611 @@
         <v>56</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>151</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
+      </c>
+      <c r="E25" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D26" t="s">
-        <v>151</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
+      <c r="D27" t="s">
+        <v>149</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B28" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" t="s">
-        <v>151</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="C28" s="7" t="s">
-        <v>69</v>
+        <v>161</v>
       </c>
       <c r="D28" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="D29" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>73</v>
-      </c>
       <c r="C30" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D31" t="s">
-        <v>151</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="D32" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>159</v>
+        <v>76</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="D34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D36" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" t="s">
+        <v>149</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="C38" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D38" t="s">
+        <v>149</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D37" t="s">
-        <v>151</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
+      <c r="B39" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="C39" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" t="s">
-        <v>151</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="D39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="C40" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D41" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>102</v>
+        <v>97</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>104</v>
-      </c>
       <c r="C43" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D45" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="C47" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="D47" t="s">
+        <v>149</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D46" t="s">
-        <v>151</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
+      <c r="B48" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="C48" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D47" t="s">
-        <v>151</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="D48" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>122</v>
+        <v>117</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D49" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D50" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D52" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="C53" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D53" t="s">
-        <v>151</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="D54" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="C55" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D55" t="s">
+        <v>149</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="D56" t="s">
+        <v>149</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D55" t="s">
-        <v>151</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
+      <c r="B57" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="C57" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C56" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D56" t="s">
-        <v>151</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>145</v>
-      </c>
       <c r="D57" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="B58" s="7" t="s">
-        <v>146</v>
-      </c>
       <c r="C58" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D58" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" t="s">
+        <v>149</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C60" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B59" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C59" s="7" t="s">
+      <c r="D60" t="s">
         <v>150</v>
       </c>
-      <c r="D59" t="s">
-        <v>152</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>157</v>
+      <c r="E60" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New: improved handling cumultive val
df_std_CF and df_std_IS properly retrieved and produced as output. Transpose df function properly defined. Minor fixes on quarto web.
</commit_message>
<xml_diff>
--- a/data/standardized_IS_CF.xlsx
+++ b/data/standardized_IS_CF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielepicheo/GitHub/SEC_data_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658C2317-2FA8-7B46-9EA4-325E0F7FB22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC50CD7-7A00-E145-B338-CAC78B669B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12680" yWindow="6920" windowWidth="21140" windowHeight="20020" xr2:uid="{4802AE4D-B274-A94A-943F-E5938A0AE0CD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="157">
   <si>
     <t>Revenue</t>
   </si>
@@ -479,18 +479,9 @@
     <t>Amount of increase (decrease) in cash and cash equivalents. Cash and cash equivalents are the amount of currency on hand as well as demand deposits with banks or financial institutions. Includes other kinds of accounts that have the general characteristics of demand deposits. Also includes short-term, highly liquid investments that are both readily convertible to known amounts of cash and so near their maturity that they present insignificant risk of changes in value because of changes in interest rates. Includes effect from exchange rate changes.</t>
   </si>
   <si>
-    <t>CashCashEquivalentsRestrictedCashAndRestrictedCashEquivalents</t>
-  </si>
-  <si>
-    <t>Amount of cash and cash equivalents, and cash and cash equivalents restricted to withdrawal or usage. Excludes amount for disposal group and discontinued operations. Cash includes, but is not limited to, currency on hand, demand deposits with banks or financial institutions, and other accounts with general characteristics of demand deposits. Cash equivalents include, but are not limited to, short-term, highly liquid investments that are both readily convertible to known amounts of cash and so near their maturity that they present insignificant risk of changes in value because of changes in interest rates.</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>Aggregated</t>
   </si>
   <si>
@@ -503,9 +494,6 @@
     <t>Financial Report</t>
   </si>
   <si>
-    <t>BS</t>
-  </si>
-  <si>
     <t>CF</t>
   </si>
   <si>
@@ -513,9 +501,6 @@
   </si>
   <si>
     <t>(Operating Activities) Change in Accounts Taxes Payable</t>
-  </si>
-  <si>
-    <t>Cash &amp; Cash Equivalent at the  end / beginning of the period</t>
   </si>
   <si>
     <t>AmortizationOfFinancingCostsAndWriteOffOfDeferredDebtIssuanceCos</t>
@@ -935,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6F0AFE-E52E-334A-8161-7EB63B8B31FB}">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -950,7 +935,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -959,10 +944,10 @@
         <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -977,10 +962,10 @@
         <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -995,10 +980,10 @@
         <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -1013,10 +998,10 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1030,10 +1015,10 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1047,10 +1032,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1064,10 +1049,10 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1081,10 +1066,10 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1098,10 +1083,10 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1115,10 +1100,10 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1132,10 +1117,10 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1149,10 +1134,10 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1166,10 +1151,10 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1183,10 +1168,10 @@
         <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1200,10 +1185,10 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1217,10 +1202,10 @@
         <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1234,10 +1219,10 @@
         <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1251,10 +1236,10 @@
         <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1268,10 +1253,10 @@
         <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1285,10 +1270,10 @@
         <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1302,10 +1287,10 @@
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E21" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1319,10 +1304,10 @@
         <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1336,10 +1321,10 @@
         <v>41</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1353,10 +1338,10 @@
         <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E24" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1364,16 +1349,16 @@
         <v>56</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E25" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1387,10 +1372,10 @@
         <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1404,10 +1389,10 @@
         <v>63</v>
       </c>
       <c r="D27" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1418,13 +1403,13 @@
         <v>65</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D28" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1438,10 +1423,10 @@
         <v>68</v>
       </c>
       <c r="D29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1455,10 +1440,10 @@
         <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1472,10 +1457,10 @@
         <v>73</v>
       </c>
       <c r="D31" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1489,15 +1474,15 @@
         <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>76</v>
@@ -1506,27 +1491,27 @@
         <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1540,10 +1525,10 @@
         <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1557,10 +1542,10 @@
         <v>82</v>
       </c>
       <c r="D36" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1574,10 +1559,10 @@
         <v>85</v>
       </c>
       <c r="D37" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1591,10 +1576,10 @@
         <v>88</v>
       </c>
       <c r="D38" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1608,10 +1593,10 @@
         <v>91</v>
       </c>
       <c r="D39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1625,10 +1610,10 @@
         <v>94</v>
       </c>
       <c r="D40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1642,10 +1627,10 @@
         <v>96</v>
       </c>
       <c r="D41" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1659,10 +1644,10 @@
         <v>99</v>
       </c>
       <c r="D42" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1676,10 +1661,10 @@
         <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1693,10 +1678,10 @@
         <v>104</v>
       </c>
       <c r="D44" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1710,10 +1695,10 @@
         <v>107</v>
       </c>
       <c r="D45" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1727,10 +1712,10 @@
         <v>110</v>
       </c>
       <c r="D46" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1744,10 +1729,10 @@
         <v>113</v>
       </c>
       <c r="D47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1761,10 +1746,10 @@
         <v>116</v>
       </c>
       <c r="D48" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1778,10 +1763,10 @@
         <v>119</v>
       </c>
       <c r="D49" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1795,10 +1780,10 @@
         <v>122</v>
       </c>
       <c r="D50" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1812,10 +1797,10 @@
         <v>125</v>
       </c>
       <c r="D51" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1829,10 +1814,10 @@
         <v>128</v>
       </c>
       <c r="D52" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1846,10 +1831,10 @@
         <v>131</v>
       </c>
       <c r="D53" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1863,10 +1848,10 @@
         <v>133</v>
       </c>
       <c r="D54" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1880,10 +1865,10 @@
         <v>136</v>
       </c>
       <c r="D55" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1897,10 +1882,10 @@
         <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1914,10 +1899,10 @@
         <v>141</v>
       </c>
       <c r="D57" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1931,10 +1916,10 @@
         <v>144</v>
       </c>
       <c r="D58" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1948,28 +1933,18 @@
         <v>146</v>
       </c>
       <c r="D59" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D60" t="s">
-        <v>150</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>155</v>
-      </c>
+      <c r="A60" s="3"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60"/>
+      <c r="E60" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>